<commit_message>
132 bridges to link
</commit_message>
<xml_diff>
--- a/EPA1352-G11-A2/check_N1_df_LB.xlsx
+++ b/EPA1352-G11-A2/check_N1_df_LB.xlsx
@@ -609,12 +609,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K3" t="n">
@@ -861,12 +861,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -2689,12 +2689,12 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K35" t="n">
@@ -7247,12 +7247,12 @@
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K103" t="n">
@@ -7440,12 +7440,12 @@
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K106" t="n">
@@ -7633,12 +7633,12 @@
       </c>
       <c r="I109" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K109" t="n">
@@ -7889,12 +7889,12 @@
       </c>
       <c r="I113" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K113" t="n">
@@ -8208,12 +8208,12 @@
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J118" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K118" t="n">
@@ -8722,12 +8722,12 @@
       </c>
       <c r="I126" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J126" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K126" t="n">
@@ -8982,12 +8982,12 @@
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J130" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K130" t="n">
@@ -9238,12 +9238,12 @@
       </c>
       <c r="I134" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J134" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K134" t="n">
@@ -9882,12 +9882,12 @@
       </c>
       <c r="I144" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J144" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K144" t="n">
@@ -10071,12 +10071,12 @@
       </c>
       <c r="I147" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J147" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K147" t="n">
@@ -10386,12 +10386,12 @@
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K152" t="n">
@@ -10449,12 +10449,12 @@
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J153" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K153" t="n">
@@ -10701,12 +10701,12 @@
       </c>
       <c r="I157" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K157" t="n">
@@ -12377,12 +12377,12 @@
       </c>
       <c r="I183" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J183" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K183" t="n">
@@ -12698,12 +12698,12 @@
       </c>
       <c r="I188" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J188" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K188" t="n">
@@ -13143,12 +13143,12 @@
       </c>
       <c r="I195" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K195" t="n">
@@ -13592,12 +13592,12 @@
       </c>
       <c r="I202" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J202" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K202" t="n">
@@ -13978,12 +13978,12 @@
       </c>
       <c r="I208" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J208" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K208" t="n">
@@ -14433,12 +14433,12 @@
       </c>
       <c r="I215" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J215" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K215" t="n">
@@ -14963,12 +14963,12 @@
       </c>
       <c r="I223" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J223" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K223" t="n">
@@ -15554,12 +15554,12 @@
       </c>
       <c r="I232" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K232" t="n">
@@ -15747,12 +15747,12 @@
       </c>
       <c r="I235" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J235" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K235" t="n">
@@ -17008,12 +17008,12 @@
       </c>
       <c r="I254" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J254" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K254" t="n">
@@ -20992,12 +20992,12 @@
       </c>
       <c r="I314" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J314" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K314" t="n">
@@ -21059,12 +21059,12 @@
       </c>
       <c r="I315" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J315" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K315" t="n">
@@ -21447,12 +21447,12 @@
       </c>
       <c r="I321" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J321" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K321" t="n">
@@ -21825,12 +21825,12 @@
       </c>
       <c r="I327" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J327" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K327" t="n">
@@ -22272,12 +22272,12 @@
       </c>
       <c r="I334" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J334" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K334" t="n">
@@ -22335,12 +22335,12 @@
       </c>
       <c r="I335" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J335" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K335" t="n">
@@ -22654,12 +22654,12 @@
       </c>
       <c r="I340" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J340" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K340" t="n">
@@ -23229,12 +23229,12 @@
       </c>
       <c r="I349" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J349" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K349" t="n">
@@ -23867,12 +23867,12 @@
       </c>
       <c r="I359" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J359" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K359" t="n">
@@ -24379,12 +24379,12 @@
       </c>
       <c r="I367" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J367" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K367" t="n">
@@ -24893,12 +24893,12 @@
       </c>
       <c r="I375" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J375" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K375" t="n">
@@ -26164,12 +26164,12 @@
       </c>
       <c r="I394" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J394" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K394" t="n">
@@ -26290,12 +26290,12 @@
       </c>
       <c r="I396" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J396" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K396" t="n">
@@ -26479,12 +26479,12 @@
       </c>
       <c r="I399" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J399" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K399" t="n">
@@ -26542,12 +26542,12 @@
       </c>
       <c r="I400" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J400" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K400" t="n">
@@ -26605,12 +26605,12 @@
       </c>
       <c r="I401" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J401" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K401" t="n">
@@ -27996,12 +27996,12 @@
       </c>
       <c r="I422" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J422" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K422" t="n">
@@ -28122,12 +28122,12 @@
       </c>
       <c r="I424" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J424" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K424" t="n">
@@ -28512,12 +28512,12 @@
       </c>
       <c r="I430" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J430" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K430" t="n">
@@ -28575,12 +28575,12 @@
       </c>
       <c r="I431" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J431" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K431" t="n">
@@ -30171,12 +30171,12 @@
       </c>
       <c r="I455" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J455" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K455" t="n">
@@ -30234,12 +30234,12 @@
       </c>
       <c r="I456" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J456" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K456" t="n">
@@ -33521,12 +33521,12 @@
       </c>
       <c r="I505" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J505" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K505" t="n">
@@ -35145,12 +35145,12 @@
       </c>
       <c r="I529" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J529" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K529" t="n">
@@ -35803,12 +35803,12 @@
       </c>
       <c r="I539" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J539" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K539" t="n">
@@ -35870,12 +35870,12 @@
       </c>
       <c r="I540" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J540" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K540" t="n">
@@ -36130,12 +36130,12 @@
       </c>
       <c r="I544" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J544" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K544" t="n">
@@ -39708,12 +39708,12 @@
       </c>
       <c r="I598" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J598" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K598" t="n">
@@ -39771,12 +39771,12 @@
       </c>
       <c r="I599" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J599" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K599" t="n">
@@ -39834,12 +39834,12 @@
       </c>
       <c r="I600" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J600" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K600" t="n">
@@ -40419,12 +40419,12 @@
       </c>
       <c r="I609" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J609" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K609" t="n">
@@ -40545,12 +40545,12 @@
       </c>
       <c r="I611" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J611" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K611" t="n">
@@ -42978,12 +42978,12 @@
       </c>
       <c r="I648" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J648" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K648" t="n">
@@ -43041,12 +43041,12 @@
       </c>
       <c r="I649" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J649" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K649" t="n">
@@ -43167,12 +43167,12 @@
       </c>
       <c r="I651" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J651" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K651" t="n">
@@ -43293,12 +43293,12 @@
       </c>
       <c r="I653" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J653" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K653" t="n">
@@ -43356,12 +43356,12 @@
       </c>
       <c r="I654" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J654" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K654" t="n">
@@ -43758,12 +43758,12 @@
       </c>
       <c r="I660" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J660" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K660" t="n">
@@ -43888,12 +43888,12 @@
       </c>
       <c r="I662" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J662" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K662" t="n">
@@ -44014,12 +44014,12 @@
       </c>
       <c r="I664" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J664" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K664" t="n">
@@ -45730,12 +45730,12 @@
       </c>
       <c r="I690" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J690" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K690" t="n">
@@ -45864,12 +45864,12 @@
       </c>
       <c r="I692" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J692" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K692" t="n">
@@ -46975,12 +46975,12 @@
       </c>
       <c r="I709" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J709" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K709" t="n">
@@ -50051,12 +50051,12 @@
       </c>
       <c r="I755" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J755" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K755" t="n">
@@ -52242,12 +52242,12 @@
       </c>
       <c r="I788" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J788" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K788" t="n">
@@ -53172,12 +53172,12 @@
       </c>
       <c r="I802" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J802" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K802" t="n">
@@ -53302,12 +53302,12 @@
       </c>
       <c r="I804" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J804" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K804" t="n">
@@ -53428,12 +53428,12 @@
       </c>
       <c r="I806" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J806" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K806" t="n">
@@ -54084,12 +54084,12 @@
       </c>
       <c r="I816" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J816" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K816" t="n">
@@ -55798,12 +55798,12 @@
       </c>
       <c r="I842" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J842" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K842" t="n">
@@ -55924,12 +55924,12 @@
       </c>
       <c r="I844" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J844" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K844" t="n">
@@ -57711,12 +57711,12 @@
       </c>
       <c r="I871" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J871" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K871" t="n">
@@ -57774,12 +57774,12 @@
       </c>
       <c r="I872" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J872" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K872" t="n">
@@ -57900,12 +57900,12 @@
       </c>
       <c r="I874" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J874" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K874" t="n">
@@ -57963,12 +57963,12 @@
       </c>
       <c r="I875" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J875" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K875" t="n">
@@ -58755,12 +58755,12 @@
       </c>
       <c r="I887" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J887" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K887" t="n">
@@ -58818,12 +58818,12 @@
       </c>
       <c r="I888" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J888" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K888" t="n">
@@ -58948,12 +58948,12 @@
       </c>
       <c r="I890" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J890" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K890" t="n">
@@ -59082,12 +59082,12 @@
       </c>
       <c r="I892" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J892" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K892" t="n">
@@ -59811,12 +59811,12 @@
       </c>
       <c r="I903" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J903" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K903" t="n">
@@ -59874,12 +59874,12 @@
       </c>
       <c r="I904" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J904" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K904" t="n">
@@ -68029,12 +68029,12 @@
       </c>
       <c r="I1025" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1025" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1025" t="n">
@@ -68092,12 +68092,12 @@
       </c>
       <c r="I1026" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1026" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1026" t="n">
@@ -68155,12 +68155,12 @@
       </c>
       <c r="I1027" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1027" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1027" t="n">
@@ -68218,12 +68218,12 @@
       </c>
       <c r="I1028" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1028" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1028" t="n">
@@ -68687,12 +68687,12 @@
       </c>
       <c r="I1035" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1035" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1035" t="n">
@@ -68817,12 +68817,12 @@
       </c>
       <c r="I1037" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1037" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1037" t="n">
@@ -70220,12 +70220,12 @@
       </c>
       <c r="I1058" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1058" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1058" t="n">
@@ -70287,12 +70287,12 @@
       </c>
       <c r="I1059" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1059" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1059" t="n">
@@ -70543,12 +70543,12 @@
       </c>
       <c r="I1063" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1063" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1063" t="n">
@@ -70610,12 +70610,12 @@
       </c>
       <c r="I1064" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1064" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1064" t="n">
@@ -70740,12 +70740,12 @@
       </c>
       <c r="I1066" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1066" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1066" t="n">
@@ -85587,12 +85587,12 @@
       </c>
       <c r="I1285" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1285" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1285" t="n">
@@ -85721,12 +85721,12 @@
       </c>
       <c r="I1287" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1287" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1287" t="n">
@@ -85851,12 +85851,12 @@
       </c>
       <c r="I1289" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1289" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1289" t="n">
@@ -85977,12 +85977,12 @@
       </c>
       <c r="I1291" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1291" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1291" t="n">
@@ -86044,12 +86044,12 @@
       </c>
       <c r="I1292" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1292" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1292" t="n">
@@ -86174,12 +86174,12 @@
       </c>
       <c r="I1294" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1294" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1294" t="n">
@@ -86237,12 +86237,12 @@
       </c>
       <c r="I1295" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1295" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1295" t="n">
@@ -86300,12 +86300,12 @@
       </c>
       <c r="I1296" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1296" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1296" t="n">
@@ -86430,12 +86430,12 @@
       </c>
       <c r="I1298" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1298" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1298" t="n">
@@ -86560,12 +86560,12 @@
       </c>
       <c r="I1300" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1300" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1300" t="n">
@@ -86623,12 +86623,12 @@
       </c>
       <c r="I1301" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1301" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1301" t="n">
@@ -86749,12 +86749,12 @@
       </c>
       <c r="I1303" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1303" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1303" t="n">
@@ -86812,12 +86812,12 @@
       </c>
       <c r="I1304" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1304" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1304" t="n">
@@ -86875,12 +86875,12 @@
       </c>
       <c r="I1305" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1305" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1305" t="n">
@@ -86942,12 +86942,12 @@
       </c>
       <c r="I1306" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1306" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1306" t="n">
@@ -87072,12 +87072,12 @@
       </c>
       <c r="I1308" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1308" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1308" t="n">
@@ -87139,12 +87139,12 @@
       </c>
       <c r="I1309" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1309" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1309" t="n">
@@ -87332,12 +87332,12 @@
       </c>
       <c r="I1312" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1312" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1312" t="n">
@@ -87395,12 +87395,12 @@
       </c>
       <c r="I1313" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1313" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1313" t="n">
@@ -87462,12 +87462,12 @@
       </c>
       <c r="I1314" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1314" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1314" t="n">
@@ -87592,12 +87592,12 @@
       </c>
       <c r="I1316" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1316" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1316" t="n">
@@ -87655,12 +87655,12 @@
       </c>
       <c r="I1317" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1317" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1317" t="n">
@@ -87718,12 +87718,12 @@
       </c>
       <c r="I1318" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1318" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1318" t="n">
@@ -87785,12 +87785,12 @@
       </c>
       <c r="I1319" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1319" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1319" t="n">
@@ -87915,12 +87915,12 @@
       </c>
       <c r="I1321" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1321" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1321" t="n">
@@ -87978,12 +87978,12 @@
       </c>
       <c r="I1322" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1322" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1322" t="n">
@@ -88108,12 +88108,12 @@
       </c>
       <c r="I1324" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1324" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1324" t="n">
@@ -88305,12 +88305,12 @@
       </c>
       <c r="I1327" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1327" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1327" t="n">
@@ -88498,12 +88498,12 @@
       </c>
       <c r="I1330" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1330" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1330" t="n">
@@ -88561,12 +88561,12 @@
       </c>
       <c r="I1331" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1331" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1331" t="n">
@@ -88691,12 +88691,12 @@
       </c>
       <c r="I1333" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1333" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1333" t="n">
@@ -88884,12 +88884,12 @@
       </c>
       <c r="I1336" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1336" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1336" t="n">
@@ -88951,12 +88951,12 @@
       </c>
       <c r="I1337" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="J1337" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="K1337" t="n">

</xml_diff>